<commit_message>
Update Figure2 readability and added new reference to ammonia in table 1
</commit_message>
<xml_diff>
--- a/table/table1_calculation_data.xlsx
+++ b/table/table1_calculation_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21948" windowHeight="8088" tabRatio="850" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="8085" tabRatio="850" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Solar, Wind Productivity" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="232">
   <si>
     <t>http://science.sciencemag.org/content/329/5993/790</t>
   </si>
@@ -1236,16 +1236,33 @@
   <si>
     <t>Ammonia from Wind Power and Direct Nitrogen Capture</t>
   </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1002/ange.201510618</t>
+  </si>
+  <si>
+    <t>Grinberg Dana, A., Elishav, O., Bardow, A., Shter, G.E., Grader, G.S., 2016. Stickstoffbasierte Kraftstoffe: eine “Power-to-Fuel-to-Power”-Analyse. Angewandte Chemie 128, 8942–8949.</t>
+  </si>
+  <si>
+    <t>Electrolysis - Ammonia Synthesis - H2 - Electricity</t>
+  </si>
+  <si>
+    <t>[23]</t>
+  </si>
+  <si>
+    <t>Electrolysis - Ammonia Synthesis - H2</t>
+  </si>
+  <si>
+    <t>Calculation from above, assuming 80% efficiency of converting Hydrogen to Electricity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1307,12 +1324,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1349,7 +1360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1358,9 +1369,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1378,7 +1386,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1675,20 +1683,20 @@
       <selection activeCell="D5" sqref="D5:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1711,7 +1719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1721,7 +1729,7 @@
       <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>42336.45</v>
       </c>
       <c r="E5" t="s">
@@ -1734,7 +1742,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1744,7 +1752,7 @@
       <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>11257.43</v>
       </c>
       <c r="E6" t="s">
@@ -1757,7 +1765,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1767,7 +1775,7 @@
       <c r="C7" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <f>8760*D5/(D6*8.76)</f>
         <v>3760.7562294413556</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -1788,7 +1796,7 @@
       <c r="C8" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <f>1/0.3</f>
         <v>3.3333333333333335</v>
       </c>
@@ -1802,7 +1810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1812,7 +1820,7 @@
       <c r="C9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>30.74</v>
       </c>
       <c r="E9" t="s">
@@ -1825,7 +1833,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1835,7 +1843,7 @@
       <c r="C10" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>19</v>
       </c>
       <c r="E10" t="s">
@@ -1848,7 +1856,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
@@ -1858,7 +1866,7 @@
       <c r="C11" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <f>8760*D9/(D10*8.76)</f>
         <v>1617.894736842105</v>
       </c>
@@ -1872,7 +1880,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
@@ -1882,7 +1890,7 @@
       <c r="C12" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <f>1/(5.9*'Energy Conversion Factors'!F8)</f>
         <v>0.41882231019538313</v>
       </c>
@@ -1896,7 +1904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -1906,7 +1914,7 @@
       <c r="C13" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <f>1/(5.9*'Energy Conversion Factors'!F8)*2</f>
         <v>0.83764462039076626</v>
       </c>
@@ -1934,20 +1942,20 @@
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>103</v>
       </c>
@@ -1970,14 +1978,14 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>122</v>
       </c>
       <c r="B7" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>0.36599999999999999</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1987,14 +1995,14 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>122</v>
       </c>
       <c r="B8" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <f>0.9*'Energy Conversion Factors'!F6</f>
         <v>0.24999993000000001</v>
       </c>
@@ -2005,14 +2013,14 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <f>490000/10^6</f>
         <v>0.49</v>
       </c>
@@ -2026,14 +2034,14 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>113</v>
       </c>
       <c r="B10" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>0.19800000000000001</v>
       </c>
       <c r="D10" t="s">
@@ -2043,14 +2051,14 @@
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>115</v>
       </c>
       <c r="B11" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <f>0.000250987654320988*1000</f>
         <v>0.25098765432098802</v>
       </c>
@@ -2061,14 +2069,14 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>113</v>
       </c>
       <c r="B12" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f>C8*C10</f>
         <v>4.9499986140000007E-2</v>
       </c>
@@ -2079,14 +2087,14 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>115</v>
       </c>
       <c r="B13" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <f>C11*C8</f>
         <v>6.2746896011111206E-2</v>
       </c>
@@ -2097,14 +2105,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>113</v>
       </c>
       <c r="B14" t="s">
         <v>141</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f>1-C8*C10</f>
         <v>0.95050001385999994</v>
       </c>
@@ -2115,14 +2123,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
       <c r="B15" t="s">
         <v>141</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <f>1-C8*C11</f>
         <v>0.93725310398888884</v>
       </c>
@@ -2133,14 +2141,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>113</v>
       </c>
       <c r="B16" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <f>1-C9*C10</f>
         <v>0.90298</v>
       </c>
@@ -2151,14 +2159,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>115</v>
       </c>
       <c r="B17" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <f>1-C9*C11</f>
         <v>0.87701604938271593</v>
       </c>
@@ -2169,14 +2177,14 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>156</v>
       </c>
       <c r="B18" t="s">
         <v>137</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <f>10^6/(150*10000)/8760</f>
         <v>7.6103500761035001E-5</v>
       </c>
@@ -2190,14 +2198,14 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>156</v>
       </c>
       <c r="B19" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <f>0.88*10^6/(18*10000)/8760</f>
         <v>5.5809233891425673E-4</v>
       </c>
@@ -2207,18 +2215,18 @@
       <c r="E19" t="s">
         <v>154</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="21" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>156</v>
       </c>
       <c r="B20" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <f>10*10^9/(10^7*10^3*8760)</f>
         <v>1.1415525114155251E-4</v>
       </c>
@@ -2229,12 +2237,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A26" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>133</v>
       </c>
@@ -2245,15 +2253,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>211</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="9">
         <f>C10/C19/10^6</f>
         <v>3.5478000000000002E-4</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="9">
         <f t="shared" ref="C28:C33" si="0">1/B28</f>
         <v>2818.6481763346296</v>
       </c>
@@ -2261,15 +2269,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>212</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="9">
         <f>C11/C19/10^6</f>
         <v>4.4972424242424309E-4</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="9">
         <f t="shared" si="0"/>
         <v>2223.5848230228594</v>
       </c>
@@ -2277,15 +2285,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>215</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="9">
         <f>C10/C18/10^6</f>
         <v>2.6017200000000001E-3</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <f t="shared" si="0"/>
         <v>384.36111495472227</v>
       </c>
@@ -2293,15 +2301,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>216</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="9">
         <f>C11/C18/10^6</f>
         <v>3.2979777777777828E-3</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="9">
         <f t="shared" si="0"/>
         <v>303.21611223038985</v>
       </c>
@@ -2309,15 +2317,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="9">
         <f>C10/C20/10^6</f>
         <v>1.7344800000000003E-3</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="9">
         <f t="shared" si="0"/>
         <v>576.54167243208326</v>
       </c>
@@ -2325,15 +2333,15 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>214</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="9">
         <f>C11/C20/10^6</f>
         <v>2.1986518518518549E-3</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <f t="shared" si="0"/>
         <v>454.82416834558489</v>
       </c>
@@ -2341,8 +2349,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2361,21 +2369,21 @@
       <selection activeCell="D4" sqref="D4:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -2407,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2417,7 +2425,7 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <f>(27*10^9)/(4.6*10^6)</f>
         <v>5869.565217391304</v>
       </c>
@@ -2441,7 +2449,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2451,7 +2459,7 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <f>(800*10^9)/(60*10^6)</f>
         <v>13333.333333333334</v>
       </c>
@@ -2465,7 +2473,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2475,7 +2483,7 @@
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>6471</v>
       </c>
       <c r="E6" t="s">
@@ -2488,7 +2496,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -2498,7 +2506,7 @@
       <c r="C7" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <f>13.6*490</f>
         <v>6664</v>
       </c>
@@ -2512,14 +2520,14 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <f>279000000000/20600000</f>
         <v>13543.68932038835</v>
       </c>
@@ -2530,7 +2538,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2540,7 +2548,7 @@
       <c r="C9" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>32</v>
       </c>
       <c r="E9" t="s">
@@ -2567,24 +2575,24 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2605,7 +2613,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2615,17 +2623,17 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>0.8</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>0.8</v>
       </c>
       <c r="F5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2635,155 +2643,186 @@
       <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>0.51</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>0.67</v>
       </c>
       <c r="F6" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>0.8</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>0.8</v>
       </c>
       <c r="F7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.8</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>0.8</v>
       </c>
       <c r="F8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <f>0.54</f>
         <v>0.54</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <v>0.6</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>0.67</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <v>0.74</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <f>3.93/12</f>
         <v>0.32750000000000001</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <f>3.93/10</f>
         <v>0.39300000000000002</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" s="11">
+        <f>0.35</f>
+        <v>0.35</v>
+      </c>
+      <c r="E12" s="11">
+        <f>0.35</f>
+        <v>0.35</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13">
+        <f>D12/0.8</f>
+        <v>0.43749999999999994</v>
+      </c>
+      <c r="E13">
+        <f>E12/0.8</f>
+        <v>0.43749999999999994</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2801,17 +2840,17 @@
       <selection activeCell="D6" sqref="D6:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2834,7 +2873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2844,18 +2883,18 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>0.27777770000000002</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>0.27777770000000002</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <f>(D6+E6)/2</f>
         <v>0.27777770000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2865,39 +2904,39 @@
       <c r="C7" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>18.399999999999999</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>21.2</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <f>(D7+E7)/2</f>
         <v>19.799999999999997</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.40468599999999999</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>0.40468599999999999</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <f>(D8+E8)/2</f>
         <v>0.40468599999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -2907,13 +2946,13 @@
       <c r="C9" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>33.299999999999997</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>35.700000000000003</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <f>(D9+E9)/2</f>
         <v>34.5</v>
       </c>
@@ -2921,7 +2960,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -2931,13 +2970,13 @@
       <c r="C10" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>18.600000000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>18.600000000000001</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <f>(D10+E10)/2</f>
         <v>18.600000000000001</v>
       </c>
@@ -2957,27 +2996,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -2997,7 +3036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>101</v>
       </c>
@@ -3007,7 +3046,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -3026,7 +3065,7 @@
         <v>66.084648162960008</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -3044,32 +3083,32 @@
         <f>'Solar, Wind Productivity'!D13*'Solar, Wind Productivity'!D11*'Technical Conversion Factors'!E5</f>
         <v>1084.1766581394591</v>
       </c>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <f>'Solar, Wind Productivity'!D8*'Solar, Wind Productivity'!D7*'Technical Conversion Factors'!D6</f>
         <v>6393.2855900503046</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <f>'Solar, Wind Productivity'!D8*'Solar, Wind Productivity'!D7*'Technical Conversion Factors'!E5</f>
         <v>10028.683278510282</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -3091,50 +3130,50 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <f>'Biomass Productivity'!D8*'Energy Conversion Factors'!F9*'Energy Conversion Factors'!F6/1000</f>
         <v>129.79365297815536</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <f>D9</f>
         <v>129.79365297815536</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="2">
@@ -3142,1146 +3181,1146 @@
         <v>221.91740971292052</v>
       </c>
       <c r="E10" s="2">
-        <f>'Solar, Wind Productivity'!$D$13*'Solar, Wind Productivity'!$D$11*'Technical Conversion Factors'!E11</f>
-        <v>532.60178331100929</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+        <f>'Solar, Wind Productivity'!$D$13*'Solar, Wind Productivity'!$D$11*'Technical Conversion Factors'!E13</f>
+        <v>592.90910992001659</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <f>'Solar, Wind Productivity'!D8*'Solar, Wind Productivity'!D7*'Technical Conversion Factors'!D11</f>
         <v>4105.4922171401467</v>
       </c>
-      <c r="E11" s="13">
-        <f>'Solar, Wind Productivity'!D8*'Solar, Wind Productivity'!D7*'Technical Conversion Factors'!E11</f>
-        <v>4926.5906605681757</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="E11" s="12">
+        <f>'Solar, Wind Productivity'!D8*'Solar, Wind Productivity'!D7*'Technical Conversion Factors'!E13</f>
+        <v>5484.4361679353096</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <f>'Biomass Productivity'!D9*'Energy Conversion Factors'!D10*'Energy Conversion Factors'!D6*'Technical Conversion Factors'!D9</f>
         <v>89.279975001600008</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <f>'Biomass Productivity'!D9*'Energy Conversion Factors'!D10*'Energy Conversion Factors'!D6*'Technical Conversion Factors'!E9</f>
         <v>99.199972224000007</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="12">
         <f>'Biomass Productivity'!D9*'Energy Conversion Factors'!D10*'Energy Conversion Factors'!D6*'Technical Conversion Factors'!D10</f>
         <v>110.77330231680001</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <f>'Biomass Productivity'!D9*'Energy Conversion Factors'!D10*'Energy Conversion Factors'!D6*'Technical Conversion Factors'!E10</f>
         <v>122.34663240960001</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="12">
         <f>(D5*'Technical Conversion Factors'!D7*'CO2-Capture'!$C$14)</f>
         <v>262.78003179000228</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <f>E5*'Technical Conversion Factors'!E7*'CO2-Capture'!$C$16</f>
         <v>783.19187101341504</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="12">
         <f>D5*'Technical Conversion Factors'!D8*'CO2-Capture'!$C$15</f>
         <v>259.11772421894466</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <f>E5*'Technical Conversion Factors'!E8*'CO2-Capture'!$C$17</f>
         <v>760.67226364353905</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <f>D6*'Technical Conversion Factors'!E7*'CO2-Capture'!$C$15</f>
         <v>4793.7014111696662</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <f>E6*'Technical Conversion Factors'!E7*'CO2-Capture'!$C$16</f>
         <v>7244.5603414633715</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="12">
         <f>D6*'Technical Conversion Factors'!D8*'CO2-Capture'!$C$15</f>
         <v>4793.7014111696662</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <f>E6*'Technical Conversion Factors'!E8*'CO2-Capture'!$C$17</f>
         <v>7036.2529515436727</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <f>'Biomass Productivity'!D5*'Energy Conversion Factors'!$F$7*'Energy Conversion Factors'!$F$6/1000</f>
         <v>73.333312800000002</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <f>D18</f>
         <v>73.333312800000002</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A20" s="17" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A20" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="str">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="str">
         <f>A3</f>
         <v xml:space="preserve">Commercially available technologies </v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="str">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="str">
         <f>A4</f>
         <v>Oil Palm</v>
       </c>
-      <c r="B23" s="12" t="str">
+      <c r="B23" s="11" t="str">
         <f>B4</f>
         <v>Transesterification</v>
       </c>
-      <c r="C23" s="12" t="str">
+      <c r="C23" s="11" t="str">
         <f>C4</f>
         <v>Biodiesel</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="24">
         <f>((D4)*100/8760)</f>
         <v>0.70367560205753421</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="24">
         <f>((E4)*100/8760)</f>
         <v>0.75439096076438372</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="str">
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="str">
         <f t="shared" ref="A24:C24" si="0">A5</f>
         <v>Electricity from Photovoltaics (PV)</v>
       </c>
-      <c r="B24" s="12" t="str">
+      <c r="B24" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Electrolysis</v>
       </c>
-      <c r="C24" s="12" t="str">
+      <c r="C24" s="11" t="str">
         <f t="shared" si="0"/>
         <v>H2</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="24">
         <f t="shared" ref="D24:E24" si="1">((D5)*100/8760)</f>
         <v>3.9449921207985446</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="24">
         <f t="shared" si="1"/>
         <v>12.376445869171906</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="str">
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="str">
         <f t="shared" ref="A25:C25" si="2">A6</f>
         <v>Electricity from Wind Power</v>
       </c>
-      <c r="B25" s="12" t="str">
+      <c r="B25" s="11" t="str">
         <f t="shared" si="2"/>
         <v>Electrolysis</v>
       </c>
-      <c r="C25" s="12" t="str">
+      <c r="C25" s="11" t="str">
         <f t="shared" si="2"/>
         <v>H2</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="24">
         <f t="shared" ref="D25:E25" si="3">((D6)*100/8760)</f>
         <v>72.982712215186126</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="24">
         <f t="shared" si="3"/>
         <v>114.48268582774294</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="str">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="str">
         <f t="shared" ref="A26:C26" si="4">A7</f>
         <v>Sugar Cane -Traditional*</v>
       </c>
-      <c r="B26" s="12" t="str">
+      <c r="B26" s="11" t="str">
         <f t="shared" si="4"/>
         <v>Fermentation</v>
       </c>
-      <c r="C26" s="12" t="str">
+      <c r="C26" s="11" t="str">
         <f t="shared" si="4"/>
         <v>Ethanol</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="24">
         <f t="shared" ref="D26:E26" si="5">((D7)*100/8760)</f>
         <v>0.36852282712924356</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="24">
         <f t="shared" si="5"/>
         <v>0.40628413281575343</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="str">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="str">
         <f t="shared" ref="A27" si="6">A8</f>
         <v>Technologies under development</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="12" t="str">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="str">
         <f>A9</f>
         <v>Algae</v>
       </c>
-      <c r="B28" s="12" t="str">
+      <c r="B28" s="11" t="str">
         <f t="shared" ref="B28:C28" si="7">B9</f>
         <v>Transesterification</v>
       </c>
-      <c r="C28" s="12" t="str">
+      <c r="C28" s="11" t="str">
         <f t="shared" si="7"/>
         <v>Biodiesel</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="24">
         <f>((D9)*100/8760)</f>
         <v>1.4816627052300841</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="24">
         <f>((E9)*100/8760)</f>
         <v>1.4816627052300841</v>
       </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="str">
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="str">
         <f t="shared" ref="A29:C29" si="8">A10</f>
         <v>Ammonia from Photovoltaics and Direct Nitrogen Capture</v>
       </c>
-      <c r="B29" s="12" t="str">
+      <c r="B29" s="11" t="str">
         <f t="shared" si="8"/>
         <v>Electrolysis, Ammonia Synthesis, and Ammonia Cracking</v>
       </c>
-      <c r="C29" s="12" t="str">
+      <c r="C29" s="11" t="str">
         <f t="shared" si="8"/>
         <v>H2</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="24">
         <f t="shared" ref="D29:E30" si="9">((D10)*100/8760)</f>
         <v>2.5333037638461247</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="24">
         <f t="shared" si="9"/>
-        <v>6.0799290332306999</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="12" t="str">
+        <v>6.7683688347033852</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="str">
         <f t="shared" ref="A30:C30" si="10">A11</f>
         <v>Ammonia from Wind Power and Direct Nitrogen Capture</v>
       </c>
-      <c r="B30" s="12" t="str">
+      <c r="B30" s="11" t="str">
         <f t="shared" si="10"/>
         <v>Electrolysis, Ammonia Synthesis, and Ammonia Cracking</v>
       </c>
-      <c r="C30" s="12" t="str">
+      <c r="C30" s="11" t="str">
         <f t="shared" si="10"/>
         <v>H2</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="24">
         <f t="shared" si="9"/>
         <v>46.866349510732263</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="24">
         <f t="shared" si="9"/>
-        <v>56.239619412878724</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="str">
+        <v>62.607718812046919</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="str">
         <f t="shared" ref="A31:C31" si="11">A12</f>
         <v>Eucalyptus</v>
       </c>
-      <c r="B31" s="12" t="str">
+      <c r="B31" s="11" t="str">
         <f t="shared" si="11"/>
         <v>Gasification and Methanol Synthesis</v>
       </c>
-      <c r="C31" s="12" t="str">
+      <c r="C31" s="11" t="str">
         <f t="shared" si="11"/>
         <v>Methanol</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="24">
         <f t="shared" ref="D31:D37" si="12">((D12)*100/8760)</f>
         <v>1.019177796821918</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="24">
         <f t="shared" ref="E31" si="13">((E12)*100/8760)</f>
         <v>1.1324197742465756</v>
       </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="24">
         <f t="shared" si="12"/>
         <v>1.2645354145753427</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="24">
         <f t="shared" ref="E32:E37" si="14">((E13)*100/8760)</f>
         <v>1.3966510549041096</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="str">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="str">
         <f t="shared" ref="A33:C33" si="15">A14</f>
         <v>Electricity from Photovoltaics and CO2 from Air Capture</v>
       </c>
-      <c r="B33" s="12" t="str">
+      <c r="B33" s="11" t="str">
         <f t="shared" si="15"/>
         <v>Electrolysis and Methanation</v>
       </c>
-      <c r="C33" s="12" t="str">
+      <c r="C33" s="11" t="str">
         <f t="shared" si="15"/>
         <v>Methane</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="24">
         <f t="shared" si="12"/>
         <v>2.9997720523972862</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="24">
         <f t="shared" si="14"/>
         <v>8.9405464727558801</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="str">
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="str">
         <f t="shared" ref="A34:C34" si="16">A15</f>
         <v>Electricity from Photovoltaics and CO2 from Air Capture</v>
       </c>
-      <c r="B34" s="12" t="str">
+      <c r="B34" s="11" t="str">
         <f t="shared" si="16"/>
         <v>Electrolysis and Methanol Synthesis</v>
       </c>
-      <c r="C34" s="12" t="str">
+      <c r="C34" s="11" t="str">
         <f t="shared" si="16"/>
         <v>Methanol</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="24">
         <f t="shared" si="12"/>
         <v>2.957964888344117</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="24">
         <f t="shared" si="14"/>
         <v>8.6834733292641442</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="str">
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="str">
         <f t="shared" ref="A35:C35" si="17">A16</f>
         <v>Electricity from Wind Power and CO2 from Air Capture</v>
       </c>
-      <c r="B35" s="12" t="str">
+      <c r="B35" s="11" t="str">
         <f t="shared" si="17"/>
         <v>Electrolysis and Methanation</v>
       </c>
-      <c r="C35" s="12" t="str">
+      <c r="C35" s="11" t="str">
         <f t="shared" si="17"/>
         <v>Methane</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="24">
         <f t="shared" si="12"/>
         <v>54.722618848968793</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="24">
         <f t="shared" si="14"/>
         <v>82.700460518988265</v>
       </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="str">
+      <c r="F35" s="15"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="str">
         <f t="shared" ref="A36:C36" si="18">A17</f>
         <v>Electricity from Wind Power and CO2 from Air Capture</v>
       </c>
-      <c r="B36" s="12" t="str">
+      <c r="B36" s="11" t="str">
         <f t="shared" si="18"/>
         <v>Electrolysis and Methanol Synthesis</v>
       </c>
-      <c r="C36" s="12" t="str">
+      <c r="C36" s="11" t="str">
         <f t="shared" si="18"/>
         <v>Methanol</v>
       </c>
-      <c r="D36" s="25">
+      <c r="D36" s="24">
         <f t="shared" si="12"/>
         <v>54.722618848968793</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="24">
         <f t="shared" si="14"/>
         <v>80.3225222778958</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="str">
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="str">
         <f t="shared" ref="A37:C37" si="19">A18</f>
         <v>Sugar Cane - 2nd Generation</v>
       </c>
-      <c r="B37" s="12" t="str">
+      <c r="B37" s="11" t="str">
         <f t="shared" si="19"/>
         <v>Hydrolysis of Bagasse and Fermentation</v>
       </c>
-      <c r="C37" s="12" t="str">
+      <c r="C37" s="11" t="str">
         <f t="shared" si="19"/>
         <v>Ethanol</v>
       </c>
-      <c r="D37" s="25">
+      <c r="D37" s="24">
         <f t="shared" si="12"/>
         <v>0.83713827397260276</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="24">
         <f t="shared" si="14"/>
         <v>0.83713827397260276</v>
       </c>
-      <c r="F37" s="13"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A40" s="17" t="s">
+      <c r="F37" s="12"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A40" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="str">
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="str">
         <f t="shared" ref="A42:A48" si="20">A22</f>
         <v xml:space="preserve">Commercially available technologies </v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="str">
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="str">
         <f t="shared" si="20"/>
         <v>Oil Palm</v>
       </c>
-      <c r="B43" s="15" t="str">
+      <c r="B43" s="14" t="str">
         <f t="shared" ref="B43:C43" si="21">B23</f>
         <v>Transesterification</v>
       </c>
-      <c r="C43" s="15" t="str">
+      <c r="C43" s="14" t="str">
         <f t="shared" si="21"/>
         <v>Biodiesel</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="24">
         <v>0</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="24">
         <v>0</v>
       </c>
-      <c r="F43" s="25">
+      <c r="F43" s="24">
         <f>1/(1/D23+E43)</f>
         <v>0.70367560205753421</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="24">
         <f>1/(1/E23+E43)</f>
         <v>0.75439096076438372</v>
       </c>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="15" t="str">
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="str">
         <f t="shared" si="20"/>
         <v>Electricity from Photovoltaics (PV)</v>
       </c>
-      <c r="B44" s="15" t="str">
+      <c r="B44" s="14" t="str">
         <f t="shared" ref="B44:C46" si="22">B24</f>
         <v>Electrolysis</v>
       </c>
-      <c r="C44" s="15" t="str">
+      <c r="C44" s="14" t="str">
         <f t="shared" si="22"/>
         <v>H2</v>
       </c>
-      <c r="D44" s="25">
+      <c r="D44" s="24">
         <v>0</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="24">
         <v>0</v>
       </c>
-      <c r="F44" s="25">
+      <c r="F44" s="24">
         <f>1/(1/D24+E44)</f>
         <v>3.9449921207985446</v>
       </c>
-      <c r="G44" s="25">
+      <c r="G44" s="24">
         <f>1/(1/E24+E44)</f>
         <v>12.376445869171906</v>
       </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="str">
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="str">
         <f t="shared" si="20"/>
         <v>Electricity from Wind Power</v>
       </c>
-      <c r="B45" s="15" t="str">
+      <c r="B45" s="14" t="str">
         <f t="shared" si="22"/>
         <v>Electrolysis</v>
       </c>
-      <c r="C45" s="15" t="str">
+      <c r="C45" s="14" t="str">
         <f t="shared" si="22"/>
         <v>H2</v>
       </c>
-      <c r="D45" s="25">
+      <c r="D45" s="24">
         <v>0</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="24">
         <v>0</v>
       </c>
-      <c r="F45" s="25">
+      <c r="F45" s="24">
         <f>1/(1/D25+E45)</f>
         <v>72.982712215186126</v>
       </c>
-      <c r="G45" s="25">
+      <c r="G45" s="24">
         <f>1/(1/E25+E45)</f>
         <v>114.48268582774294</v>
       </c>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="str">
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="str">
         <f t="shared" si="20"/>
         <v>Sugar Cane -Traditional*</v>
       </c>
-      <c r="B46" s="15" t="str">
+      <c r="B46" s="14" t="str">
         <f t="shared" si="22"/>
         <v>Fermentation</v>
       </c>
-      <c r="C46" s="15" t="str">
+      <c r="C46" s="14" t="str">
         <f t="shared" si="22"/>
         <v>Ethanol</v>
       </c>
-      <c r="D46" s="25">
+      <c r="D46" s="24">
         <v>0</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="24">
         <v>0</v>
       </c>
-      <c r="F46" s="25">
+      <c r="F46" s="24">
         <f>1/(1/D26+E46)</f>
         <v>0.36852282712924356</v>
       </c>
-      <c r="G46" s="25">
+      <c r="G46" s="24">
         <f>1/(1/E26+E46)</f>
         <v>0.40628413281575343</v>
       </c>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="18" t="str">
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="str">
         <f t="shared" si="20"/>
         <v>Technologies under development</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="str">
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="str">
         <f t="shared" si="20"/>
         <v>Algae</v>
       </c>
-      <c r="B48" s="15" t="str">
+      <c r="B48" s="14" t="str">
         <f>B28</f>
         <v>Transesterification</v>
       </c>
-      <c r="C48" s="15" t="str">
+      <c r="C48" s="14" t="str">
         <f>C28</f>
         <v>Biodiesel</v>
       </c>
-      <c r="D48" s="25">
+      <c r="D48" s="24">
         <v>0</v>
       </c>
-      <c r="E48" s="26">
+      <c r="E48" s="25">
         <v>0</v>
       </c>
-      <c r="F48" s="25">
+      <c r="F48" s="24">
         <f t="shared" ref="F48" si="23">1/(1/D28+E48)</f>
         <v>1.4816627052300841</v>
       </c>
-      <c r="G48" s="25">
+      <c r="G48" s="24">
         <f>1/(1/E28+E48)</f>
         <v>1.4816627052300841</v>
       </c>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="str">
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="str">
         <f t="shared" ref="A49:C49" si="24">A29</f>
         <v>Ammonia from Photovoltaics and Direct Nitrogen Capture</v>
       </c>
-      <c r="B49" s="15" t="str">
+      <c r="B49" s="14" t="str">
         <f t="shared" si="24"/>
         <v>Electrolysis, Ammonia Synthesis, and Ammonia Cracking</v>
       </c>
-      <c r="C49" s="15" t="str">
+      <c r="C49" s="14" t="str">
         <f t="shared" si="24"/>
         <v>H2</v>
       </c>
-      <c r="D49" s="25">
+      <c r="D49" s="24">
         <v>0</v>
       </c>
-      <c r="E49" s="26">
+      <c r="E49" s="25">
         <v>0</v>
       </c>
-      <c r="F49" s="25">
+      <c r="F49" s="24">
         <f t="shared" ref="F49:F50" si="25">1/(1/D29+E49)</f>
         <v>2.5333037638461247</v>
       </c>
-      <c r="G49" s="25">
+      <c r="G49" s="24">
         <f t="shared" ref="G49:G50" si="26">1/(1/E29+E49)</f>
-        <v>6.0799290332306999</v>
-      </c>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="15" t="str">
+        <v>6.7683688347033852</v>
+      </c>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="str">
         <f t="shared" ref="A50:C50" si="27">A30</f>
         <v>Ammonia from Wind Power and Direct Nitrogen Capture</v>
       </c>
-      <c r="B50" s="15" t="str">
+      <c r="B50" s="14" t="str">
         <f t="shared" si="27"/>
         <v>Electrolysis, Ammonia Synthesis, and Ammonia Cracking</v>
       </c>
-      <c r="C50" s="15" t="str">
+      <c r="C50" s="14" t="str">
         <f t="shared" si="27"/>
         <v>H2</v>
       </c>
-      <c r="D50" s="25">
+      <c r="D50" s="24">
         <v>0</v>
       </c>
-      <c r="E50" s="26">
+      <c r="E50" s="25">
         <v>0</v>
       </c>
-      <c r="F50" s="25">
+      <c r="F50" s="24">
         <f t="shared" si="25"/>
         <v>46.866349510732263</v>
       </c>
-      <c r="G50" s="25">
+      <c r="G50" s="24">
         <f t="shared" si="26"/>
-        <v>56.239619412878717</v>
-      </c>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="12" t="s">
+        <v>62.607718812046912</v>
+      </c>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D51" s="25">
+      <c r="D51" s="24">
         <v>0</v>
       </c>
-      <c r="E51" s="26">
+      <c r="E51" s="25">
         <v>0</v>
       </c>
-      <c r="F51" s="25">
+      <c r="F51" s="24">
         <f>1/(1/D32+E51)</f>
         <v>1.2645354145753427</v>
       </c>
-      <c r="G51" s="25">
+      <c r="G51" s="24">
         <f>1/(1/E32+E51)</f>
         <v>1.3966510549041096</v>
       </c>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="15" t="str">
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="str">
         <f>A31</f>
         <v>Eucalyptus</v>
       </c>
-      <c r="B52" s="15" t="str">
+      <c r="B52" s="14" t="str">
         <f>B31</f>
         <v>Gasification and Methanol Synthesis</v>
       </c>
-      <c r="C52" s="15" t="str">
+      <c r="C52" s="14" t="str">
         <f>C31</f>
         <v>Methanol</v>
       </c>
-      <c r="D52" s="25">
+      <c r="D52" s="24">
         <v>0</v>
       </c>
-      <c r="E52" s="26">
+      <c r="E52" s="25">
         <v>0</v>
       </c>
-      <c r="F52" s="25">
+      <c r="F52" s="24">
         <f>1/(1/D31+E52)</f>
         <v>1.019177796821918</v>
       </c>
-      <c r="G52" s="25">
+      <c r="G52" s="24">
         <f>1/(1/E31+E52)</f>
         <v>1.1324197742465756</v>
       </c>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="15" t="str">
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="str">
         <f t="shared" ref="A53:C57" si="28">A33</f>
         <v>Electricity from Photovoltaics and CO2 from Air Capture</v>
       </c>
-      <c r="B53" s="15" t="str">
+      <c r="B53" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Electrolysis and Methanation</v>
       </c>
-      <c r="C53" s="15" t="str">
+      <c r="C53" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Methane</v>
       </c>
-      <c r="D53" s="25">
+      <c r="D53" s="24">
         <f>'CO2-Capture'!B32</f>
         <v>1.7344800000000003E-3</v>
       </c>
-      <c r="E53" s="26">
+      <c r="E53" s="25">
         <f>'CO2-Capture'!B28</f>
         <v>3.5478000000000002E-4</v>
       </c>
-      <c r="F53" s="25">
+      <c r="F53" s="24">
         <f>1/(1/D33+E53)</f>
         <v>2.9965829116784777</v>
       </c>
-      <c r="G53" s="25">
+      <c r="G53" s="24">
         <f>1/(1/E33+E53)</f>
         <v>8.9122773788148972</v>
       </c>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="str">
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Electricity from Photovoltaics and CO2 from Air Capture</v>
       </c>
-      <c r="B54" s="15" t="str">
+      <c r="B54" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Electrolysis and Methanol Synthesis</v>
       </c>
-      <c r="C54" s="15" t="str">
+      <c r="C54" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Methanol</v>
       </c>
-      <c r="D54" s="25">
+      <c r="D54" s="24">
         <f>'CO2-Capture'!B33</f>
         <v>2.1986518518518549E-3</v>
       </c>
-      <c r="E54" s="26">
+      <c r="E54" s="25">
         <f>'CO2-Capture'!B29</f>
         <v>4.4972424242424309E-4</v>
       </c>
-      <c r="F54" s="25">
+      <c r="F54" s="24">
         <f>1/(1/D34+E54)</f>
         <v>2.9540352282773168</v>
       </c>
-      <c r="G54" s="25">
+      <c r="G54" s="24">
         <f>1/(1/E34+E54)</f>
         <v>8.6496948138485639</v>
       </c>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="15" t="str">
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Electricity from Wind Power and CO2 from Air Capture</v>
       </c>
-      <c r="B55" s="15" t="str">
+      <c r="B55" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Electrolysis and Methanation</v>
       </c>
-      <c r="C55" s="15" t="str">
+      <c r="C55" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Methane</v>
       </c>
-      <c r="D55" s="25">
+      <c r="D55" s="24">
         <f>'CO2-Capture'!B32</f>
         <v>1.7344800000000003E-3</v>
       </c>
-      <c r="E55" s="26">
+      <c r="E55" s="25">
         <f>'CO2-Capture'!B28</f>
         <v>3.5478000000000002E-4</v>
       </c>
-      <c r="F55" s="25">
+      <c r="F55" s="24">
         <f>1/(1/D35+E55)</f>
         <v>53.680440436524059</v>
       </c>
-      <c r="G55" s="25">
+      <c r="G55" s="24">
         <f>1/(1/E35+E55)</f>
         <v>80.343154649856402</v>
       </c>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="15" t="str">
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Electricity from Wind Power and CO2 from Air Capture</v>
       </c>
-      <c r="B56" s="15" t="str">
+      <c r="B56" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Electrolysis and Methanol Synthesis</v>
       </c>
-      <c r="C56" s="15" t="str">
+      <c r="C56" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Methanol</v>
       </c>
-      <c r="D56" s="25">
+      <c r="D56" s="24">
         <f>'CO2-Capture'!B33</f>
         <v>2.1986518518518549E-3</v>
       </c>
-      <c r="E56" s="26">
+      <c r="E56" s="25">
         <f>'CO2-Capture'!B29</f>
         <v>4.4972424242424309E-4</v>
       </c>
-      <c r="F56" s="25">
+      <c r="F56" s="24">
         <f>1/(1/D36+E56)</f>
         <v>53.408237410075181</v>
       </c>
-      <c r="G56" s="25">
+      <c r="G56" s="24">
         <f>1/(1/E36+E56)</f>
         <v>77.522189357284859</v>
       </c>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="15" t="str">
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Sugar Cane - 2nd Generation</v>
       </c>
-      <c r="B57" s="15" t="str">
+      <c r="B57" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Hydrolysis of Bagasse and Fermentation</v>
       </c>
-      <c r="C57" s="15" t="str">
+      <c r="C57" s="14" t="str">
         <f t="shared" si="28"/>
         <v>Ethanol</v>
       </c>
-      <c r="D57" s="25">
+      <c r="D57" s="24">
         <v>0</v>
       </c>
-      <c r="E57" s="26">
+      <c r="E57" s="25">
         <v>0</v>
       </c>
-      <c r="F57" s="25">
+      <c r="F57" s="24">
         <f>1/(1/D37+E57)</f>
         <v>0.83713827397260288</v>
       </c>
-      <c r="G57" s="25">
+      <c r="G57" s="24">
         <f>1/(1/E37+E57)</f>
         <v>0.83713827397260288</v>
       </c>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-    </row>
-    <row r="59" spans="1:9" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+    </row>
+    <row r="59" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A59" s="3" t="s">
         <v>159</v>
       </c>
@@ -4290,7 +4329,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f t="shared" ref="A60:A67" si="29">A41</f>
         <v>Primary Resource</v>
@@ -4303,26 +4342,26 @@
         <f t="shared" si="30"/>
         <v>Product</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="F60" s="11" t="s">
+      <c r="F60" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="G60" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f t="shared" si="29"/>
         <v xml:space="preserve">Commercially available technologies </v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f t="shared" si="29"/>
         <v>Oil Palm</v>
@@ -4352,7 +4391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f t="shared" si="29"/>
         <v>Electricity from Photovoltaics (PV)</v>
@@ -4382,7 +4421,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f t="shared" si="29"/>
         <v>Electricity from Wind Power</v>
@@ -4412,7 +4451,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f t="shared" si="29"/>
         <v>Sugar Cane -Traditional*</v>
@@ -4443,7 +4482,7 @@
       </c>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f t="shared" si="29"/>
         <v>Technologies under development</v>
@@ -4453,7 +4492,7 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f t="shared" si="29"/>
         <v>Algae</v>
@@ -4483,7 +4522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f t="shared" ref="A68:C68" si="36">A49</f>
         <v>Ammonia from Photovoltaics and Direct Nitrogen Capture</v>
@@ -4502,7 +4541,7 @@
       </c>
       <c r="E68" s="2">
         <f t="shared" si="37"/>
-        <v>53.3</v>
+        <v>59.3</v>
       </c>
       <c r="F68" s="2">
         <f t="shared" si="34"/>
@@ -4510,10 +4549,10 @@
       </c>
       <c r="G68" s="2">
         <f t="shared" si="35"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f t="shared" ref="A69:C69" si="38">A50</f>
         <v>Ammonia from Wind Power and Direct Nitrogen Capture</v>
@@ -4532,7 +4571,7 @@
       </c>
       <c r="E69" s="2">
         <f t="shared" si="39"/>
-        <v>492.66</v>
+        <v>548.44000000000005</v>
       </c>
       <c r="F69" s="2">
         <f t="shared" si="34"/>
@@ -4540,10 +4579,10 @@
       </c>
       <c r="G69" s="2">
         <f t="shared" si="35"/>
-        <v>490</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f t="shared" ref="A70:C70" si="40">A51</f>
         <v>Eucalyptus</v>
@@ -4573,7 +4612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f t="shared" ref="A71:C71" si="42">A52</f>
         <v>Eucalyptus</v>
@@ -4603,7 +4642,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f t="shared" ref="A72:C72" si="43">A53</f>
         <v>Electricity from Photovoltaics and CO2 from Air Capture</v>
@@ -4633,7 +4672,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f t="shared" ref="A73:C73" si="44">A54</f>
         <v>Electricity from Photovoltaics and CO2 from Air Capture</v>
@@ -4663,7 +4702,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f t="shared" ref="A74:C74" si="45">A55</f>
         <v>Electricity from Wind Power and CO2 from Air Capture</v>
@@ -4693,7 +4732,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f t="shared" ref="A75:C75" si="46">A56</f>
         <v>Electricity from Wind Power and CO2 from Air Capture</v>
@@ -4723,7 +4762,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f t="shared" ref="A76:C76" si="47">A57</f>
         <v>Sugar Cane - 2nd Generation</v>
@@ -4753,7 +4792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>162</v>
       </c>
@@ -4772,21 +4811,21 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="90.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -4800,7 +4839,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4811,7 +4850,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4822,7 +4861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4833,197 +4872,197 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>189</v>
       </c>
       <c r="C7" t="s">
         <v>198</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>207</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="22" t="s">
         <v>190</v>
       </c>
       <c r="D9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>203</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>191</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>192</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>193</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>194</v>
       </c>
       <c r="D14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>195</v>
       </c>
       <c r="D15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="20" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>208</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5034,7 +5073,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5044,40 +5083,49 @@
       <c r="D24" t="s">
         <v>218</v>
       </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D25" t="s">
+        <v>226</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>